<commit_message>
update hoa don loi template
</commit_message>
<xml_diff>
--- a/API/wwwroot/docs/HoaDonDienTu/HOA_DON_LOI.xlsx
+++ b/API/wwwroot/docs/HoaDonDienTu/HOA_DON_LOI.xlsx
@@ -1,100 +1,120 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GIT\bill-back-end\API\wwwroot\docs\HoaDonDienTu\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\bill-back-end\API\wwwroot\docs\HoaDonDienTu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B5E170A2-5C50-446D-9FF7-9BA3DC9B11B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AD0AB68-EAA1-4EB3-9D19-6A226FB4C40D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{57956EFA-239D-4835-BBF4-D46DE4717CF5}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>STT</t>
   </si>
   <si>
+    <t>Ngày hóa đơn</t>
+  </si>
+  <si>
+    <t>Số hóa đơn</t>
+  </si>
+  <si>
+    <t>Ký hiệu mẫu số hóa đơn</t>
+  </si>
+  <si>
+    <t>Ký hiệu hóa đơn</t>
+  </si>
+  <si>
+    <t>Mã khách hàng</t>
+  </si>
+  <si>
+    <t>Tên khách hàng</t>
+  </si>
+  <si>
+    <t>Mã số thuế</t>
+  </si>
+  <si>
+    <t>Người mua hàng</t>
+  </si>
+  <si>
+    <t>Loại tiền</t>
+  </si>
+  <si>
+    <t>Tổng tiền thanh toán</t>
+  </si>
+  <si>
     <t>Tình trạng</t>
-  </si>
-  <si>
-    <t>Trạng thái hóa đơn</t>
-  </si>
-  <si>
-    <t>Loại hóa đơn</t>
-  </si>
-  <si>
-    <t>Mẫu số hóa đơn</t>
-  </si>
-  <si>
-    <t>Ký hiệu hóa đơn</t>
-  </si>
-  <si>
-    <t>Ngày hóa đơn</t>
-  </si>
-  <si>
-    <t>Số hóa đơn</t>
-  </si>
-  <si>
-    <t>Mã khách hàng</t>
-  </si>
-  <si>
-    <t>Tên khách hàng</t>
-  </si>
-  <si>
-    <t>Mã số thuế</t>
-  </si>
-  <si>
-    <t>Người mua hàng</t>
-  </si>
-  <si>
-    <t>Loại tiền</t>
-  </si>
-  <si>
-    <t>Tổng tiền thanh toán</t>
-  </si>
-  <si>
-    <t>Ngày lập</t>
-  </si>
-  <si>
-    <t>Người lập</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -103,18 +123,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -124,35 +138,55 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color theme="4"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color theme="4"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color theme="4"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="hair">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{1BAE8359-BB78-40ED-8F2F-283B0F1F8CA0}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -463,30 +497,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7A02382-5C58-40A1-9F1A-FD828D0E77AC}">
-  <dimension ref="A1:P2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="27.140625" customWidth="1"/>
-    <col min="3" max="3" width="27.5703125" customWidth="1"/>
-    <col min="4" max="4" width="24.7109375" customWidth="1"/>
-    <col min="5" max="5" width="19.7109375" customWidth="1"/>
-    <col min="6" max="6" width="20.28515625" customWidth="1"/>
-    <col min="7" max="7" width="20.5703125" customWidth="1"/>
-    <col min="8" max="8" width="22" customWidth="1"/>
-    <col min="9" max="9" width="21.85546875" customWidth="1"/>
-    <col min="10" max="10" width="33.85546875" customWidth="1"/>
-    <col min="11" max="14" width="21.85546875" customWidth="1"/>
-    <col min="15" max="15" width="21.5703125" customWidth="1"/>
-    <col min="16" max="16" width="20.42578125" customWidth="1"/>
+    <col min="2" max="2" width="16.875" customWidth="1"/>
+    <col min="3" max="3" width="14.875" customWidth="1"/>
+    <col min="4" max="4" width="22" customWidth="1"/>
+    <col min="5" max="5" width="16.5" customWidth="1"/>
+    <col min="6" max="6" width="18.5" customWidth="1"/>
+    <col min="7" max="7" width="30" customWidth="1"/>
+    <col min="8" max="8" width="19.25" customWidth="1"/>
+    <col min="9" max="9" width="31.875" customWidth="1"/>
+    <col min="10" max="10" width="10.5" customWidth="1"/>
+    <col min="11" max="11" width="21.125" customWidth="1"/>
+    <col min="12" max="12" width="34" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -523,20 +556,8 @@
       <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>15</v>
-      </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -548,11 +569,7 @@
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-      <c r="P2" s="3"/>
+      <c r="L2" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update template hoa don loi
</commit_message>
<xml_diff>
--- a/API/wwwroot/docs/HoaDonDienTu/HOA_DON_LOI.xlsx
+++ b/API/wwwroot/docs/HoaDonDienTu/HOA_DON_LOI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\bill-back-end\API\wwwroot\docs\HoaDonDienTu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AD0AB68-EAA1-4EB3-9D19-6A226FB4C40D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED852EA2-126A-4B54-A769-238C6F012E89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -68,7 +68,7 @@
     <t>Tổng tiền thanh toán</t>
   </si>
   <si>
-    <t>Tình trạng</t>
+    <t>Mô tả lỗi/Hướng dẫn xử lý</t>
   </si>
 </sst>
 </file>
@@ -500,9 +500,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>